<commit_message>
Fixed Alert to STU3 Updated Progress xlsx
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1055,9 +1055,11 @@
         <v>29</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="25"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7"/>
       <c r="G18" s="25" t="s">
         <v>57</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="21"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25" t="s">

</xml_diff>

<commit_message>
Updated Progress - BGZ to FHIR.xlsx
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
   <si>
     <t>Patiënt</t>
   </si>
@@ -124,9 +125,6 @@
     <t>RelatedPerson</t>
   </si>
   <si>
-    <t xml:space="preserve">Immunization </t>
-  </si>
-  <si>
     <t>NutritionOrder</t>
   </si>
   <si>
@@ -187,9 +185,6 @@
     <t>gForge #13201</t>
   </si>
   <si>
-    <t>ZIB-438 / ZIB-526 / gForge #12798</t>
-  </si>
-  <si>
     <t>ZIB-568 / gForge #12799 / gForge #12800</t>
   </si>
   <si>
@@ -209,13 +204,178 @@
   </si>
   <si>
     <t>Profile based validated - alfa</t>
+  </si>
+  <si>
+    <t>Immunization / ImmunizationRecommendation</t>
+  </si>
+  <si>
+    <t>ZIB-438 / ZIB-526 / ZIB-591 / ZIB-592 / ZIB-593 / gForge #12798</t>
+  </si>
+  <si>
+    <t>Discussed</t>
+  </si>
+  <si>
+    <t>HL7 WGM 30-03</t>
+  </si>
+  <si>
+    <t>HL7 WGM 31-03</t>
+  </si>
+  <si>
+    <t>WebEx 24-04</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ZIB</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIB-591 </t>
+  </si>
+  <si>
+    <t>ZIB-592</t>
+  </si>
+  <si>
+    <t>ZIB-593</t>
+  </si>
+  <si>
+    <t>ZIB-594</t>
+  </si>
+  <si>
+    <t>ZIB-595</t>
+  </si>
+  <si>
+    <t>Vaccination</t>
+  </si>
+  <si>
+    <t>Uitbreiding references (naast Conditie::Concern)</t>
+  </si>
+  <si>
+    <t>Constraint in keuze box verwijderen</t>
+  </si>
+  <si>
+    <t>Herzie Alert codelijsten</t>
+  </si>
+  <si>
+    <t>Granulariteit ZIB Vaccinatie – GewensteDatumHervaccinatie</t>
+  </si>
+  <si>
+    <t>Informatiebron vaccinatie</t>
+  </si>
+  <si>
+    <t>#10369</t>
+  </si>
+  <si>
+    <t>ZIB-470</t>
+  </si>
+  <si>
+    <t>ZIB-562</t>
+  </si>
+  <si>
+    <t>ZIB-475</t>
+  </si>
+  <si>
+    <t>ZIB-561</t>
+  </si>
+  <si>
+    <t>#13201</t>
+  </si>
+  <si>
+    <t>ZIB-438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIB-526 </t>
+  </si>
+  <si>
+    <t>ZIB-568</t>
+  </si>
+  <si>
+    <t>#12799</t>
+  </si>
+  <si>
+    <t>#12800</t>
+  </si>
+  <si>
+    <t>ZIB-570</t>
+  </si>
+  <si>
+    <t>Funct. OfMentaleStatus        </t>
+  </si>
+  <si>
+    <t>Bouwsteen Alert aanpassen om het probleem als reden van het alert door te geven zonder dat het naar het concept concern wordt verwezen.</t>
+  </si>
+  <si>
+    <t>Toevoegen EindDatum bij zibs die ook BeginDatum kennen</t>
+  </si>
+  <si>
+    <t>Context reference Zorgaanbieder ontbreekt</t>
+  </si>
+  <si>
+    <t>ZIB betaler: banknaam onnodig verplicht</t>
+  </si>
+  <si>
+    <t>Terminologiekoppeling Alcoholgebruik</t>
+  </si>
+  <si>
+    <t>Behandeld</t>
+  </si>
+  <si>
+    <t>Terminologiekoppeling Tabakgebruik</t>
+  </si>
+  <si>
+    <t>Terminologiekoppeling Drugsgebruik</t>
+  </si>
+  <si>
+    <t>Terminologiekoppeling Woonsituatie</t>
+  </si>
+  <si>
+    <t>Example Instances niet correct</t>
+  </si>
+  <si>
+    <t>Terminologiekoppeling FunctioneleOfMentaleStatus</t>
+  </si>
+  <si>
+    <t>Extend AllergyIntoleranceCertainty with Unknown, Ruled Out, and Possible </t>
+  </si>
+  <si>
+    <t>Condition Xpath constraint con-4 is not correct </t>
+  </si>
+  <si>
+    <t>DeviceUseStatement indication reference </t>
+  </si>
+  <si>
+    <t>DeviceUseStatement healthcareProvider reference </t>
+  </si>
+  <si>
+    <t>ZIB-567 / ZIB-594 / ZIB-595</t>
+  </si>
+  <si>
+    <t>gForge #13155</t>
+  </si>
+  <si>
+    <t>#13155</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Encounter.serviceProvider use and description not clear </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -248,6 +408,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -409,7 +576,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -460,6 +627,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -764,48 +935,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="11" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="13" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="73.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H1" s="35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -819,8 +994,11 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H2" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
@@ -834,13 +1012,16 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="25"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H3" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="7"/>
@@ -849,8 +1030,11 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H4" s="33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
@@ -864,10 +1048,11 @@
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>31</v>
@@ -879,10 +1064,11 @@
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="25" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
@@ -894,8 +1080,9 @@
       <c r="E7" s="21"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
@@ -907,8 +1094,9 @@
       <c r="E8" s="21"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -920,10 +1108,11 @@
       <c r="E9" s="21"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -937,10 +1126,11 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
@@ -954,10 +1144,11 @@
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
@@ -971,10 +1162,11 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -988,8 +1180,9 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>10</v>
       </c>
@@ -1003,10 +1196,11 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
@@ -1014,12 +1208,19 @@
         <v>16</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="D15" s="7"/>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
@@ -1027,14 +1228,19 @@
         <v>28</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7"/>
       <c r="G16" s="25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>20</v>
       </c>
@@ -1046,8 +1252,11 @@
       <c r="E17" s="21"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H17" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>19</v>
       </c>
@@ -1061,81 +1270,99 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="H18" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="25"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7"/>
       <c r="G19" s="25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="H19" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="25"/>
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="25"/>
       <c r="E21" s="21"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="25"/>
       <c r="E22" s="21"/>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H22" s="33"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="25"/>
       <c r="E23" s="21"/>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H23" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1149,43 +1376,46 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="1:8" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="25"/>
       <c r="E25" s="21"/>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="26"/>
       <c r="E26" s="23"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H26" s="34"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>13</v>
@@ -1193,7 +1423,7 @@
       <c r="C29" s="17"/>
       <c r="D29" s="12"/>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
@@ -1267,6 +1497,264 @@
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Progress xlsx and mapping dietaryRecommendations
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="124">
   <si>
     <t>Patiënt</t>
   </si>
@@ -113,9 +113,6 @@
     <t>AllergyIntolerance</t>
   </si>
   <si>
-    <t>Medication / MedicationAdministration / MedicationDispense / MedicationOrder / MedicationStatement / Substance / Timing</t>
-  </si>
-  <si>
     <t>Observation / DiagnosticReport / Specimen</t>
   </si>
   <si>
@@ -131,18 +128,6 @@
     <t xml:space="preserve">Device / DeviceUseStatement  </t>
   </si>
   <si>
-    <t>Terminology needed. ZIB-470</t>
-  </si>
-  <si>
-    <t>Terminology needed. ZIB-562</t>
-  </si>
-  <si>
-    <t>Terminology needed. ZIB-475</t>
-  </si>
-  <si>
-    <t>Terminology needed. ZIB-561</t>
-  </si>
-  <si>
     <t>ZIB-567</t>
   </si>
   <si>
@@ -182,39 +167,21 @@
     <t>Profiled</t>
   </si>
   <si>
-    <t>gForge #13201</t>
-  </si>
-  <si>
-    <t>ZIB-568 / gForge #12799 / gForge #12800</t>
-  </si>
-  <si>
     <t>Extension in nl-core-patient.</t>
   </si>
   <si>
     <t>Examples? (number)</t>
   </si>
   <si>
-    <t>Gforge #10369</t>
-  </si>
-  <si>
     <t>Practitioner / PratitionerRole</t>
   </si>
   <si>
-    <t>Need to add an invariant - ZIB-570</t>
-  </si>
-  <si>
     <t>Profile based validated - alfa</t>
   </si>
   <si>
     <t>Immunization / ImmunizationRecommendation</t>
   </si>
   <si>
-    <t>ZIB-438 / ZIB-526 / ZIB-591 / ZIB-592 / ZIB-593 / gForge #12798</t>
-  </si>
-  <si>
-    <t>Discussed</t>
-  </si>
-  <si>
     <t>HL7 WGM 30-03</t>
   </si>
   <si>
@@ -356,12 +323,6 @@
     <t>DeviceUseStatement healthcareProvider reference </t>
   </si>
   <si>
-    <t>ZIB-567 / ZIB-594 / ZIB-595</t>
-  </si>
-  <si>
-    <t>gForge #13155</t>
-  </si>
-  <si>
     <t>#13155</t>
   </si>
   <si>
@@ -369,13 +330,71 @@
   </si>
   <si>
     <t>Encounter.serviceProvider use and description not clear </t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>#13290</t>
+  </si>
+  <si>
+    <t>Immunization – Organization reference?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIB-594 </t>
+  </si>
+  <si>
+    <t>#13159</t>
+  </si>
+  <si>
+    <t>Add a reference to practitionerRole in procedureRequest </t>
+  </si>
+  <si>
+    <t>Validator does not correctly validate the performer slicing.</t>
+  </si>
+  <si>
+    <t>Validator does not correctly validate the valuesets binded to sliced contact element</t>
+  </si>
+  <si>
+    <t>Extensions on derived nl-core-patient are correctly validated</t>
+  </si>
+  <si>
+    <t>#13294</t>
+  </si>
+  <si>
+    <t>Add a note element to NutritionOrder </t>
+  </si>
+  <si>
+    <t>Not everything is specified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not everything is profiled yet, example can be improved. This whole recource needs attention! gForge #13294 - </t>
+  </si>
+  <si>
+    <t>Issues? FHIR / ZIB</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Need to add an invariant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Current Procedure.code valueset misses valid OID for system. The ZIB 3.0 valueset has fixed this. (ZIB-401 CBV Verrichtingen mist geldig OID)</t>
+  </si>
+  <si>
+    <t>Medication / MedicationAdministration / MedicationDispense / MedicationOrder / MedicationStatement  / Timing / DosalInsructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -415,6 +434,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -576,7 +601,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -631,6 +656,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -935,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -946,41 +980,45 @@
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="41.140625" style="10" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" style="13" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.5703125" style="13" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -992,18 +1030,21 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="36" t="s">
+        <v>112</v>
+      </c>
       <c r="G2" s="24"/>
-      <c r="H2" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H2" s="25"/>
+      <c r="I2" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="7"/>
@@ -1012,16 +1053,17 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="25"/>
-      <c r="H3" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H3" s="25"/>
+      <c r="I3" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="7"/>
@@ -1030,16 +1072,17 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="25"/>
-      <c r="H4" s="33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H4" s="25"/>
+      <c r="I4" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="7"/>
@@ -1048,11 +1091,12 @@
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="25"/>
-      <c r="H5" s="33"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H5" s="25"/>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>31</v>
@@ -1063,40 +1107,43 @@
         <v>1</v>
       </c>
       <c r="F6" s="15"/>
-      <c r="G6" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="33"/>
-    </row>
-    <row r="7" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="25"/>
+      <c r="H6" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="33"/>
+    </row>
+    <row r="7" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="25"/>
       <c r="E7" s="21"/>
       <c r="F7" s="25"/>
       <c r="G7" s="25"/>
-      <c r="H7" s="33"/>
-    </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H7" s="25"/>
+      <c r="I7" s="33"/>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="20"/>
+        <v>122</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="25"/>
       <c r="E8" s="21"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="33"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H8" s="25"/>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -1108,11 +1155,12 @@
       <c r="E9" s="21"/>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="33"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="H9" s="25"/>
+      <c r="I9" s="33"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -1125,12 +1173,13 @@
         <v>1</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="33"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G10" s="25"/>
+      <c r="H10" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="33"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
@@ -1143,12 +1192,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="15"/>
-      <c r="G11" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="33"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G11" s="25"/>
+      <c r="H11" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
@@ -1161,12 +1211,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="33"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G12" s="25"/>
+      <c r="H12" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" s="33"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>11</v>
       </c>
@@ -1180,9 +1231,10 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="25"/>
-      <c r="H13" s="33"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H13" s="25"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>10</v>
       </c>
@@ -1195,12 +1247,13 @@
         <v>1</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="33"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G14" s="25"/>
+      <c r="H14" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="33"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>17</v>
       </c>
@@ -1213,14 +1266,15 @@
         <v>2</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G15" s="25"/>
+      <c r="H15" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I15" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
@@ -1233,14 +1287,15 @@
         <v>2</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G16" s="25"/>
+      <c r="H16" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>20</v>
       </c>
@@ -1248,15 +1303,24 @@
         <v>30</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>19</v>
       </c>
@@ -1269,19 +1333,20 @@
         <v>1</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G18" s="25"/>
+      <c r="H18" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="7"/>
@@ -1289,19 +1354,20 @@
         <v>2</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="H19" s="33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="G19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="7"/>
@@ -1309,60 +1375,76 @@
         <v>2</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="33"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="33"/>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D21" s="7"/>
+      <c r="E21" s="4">
+        <v>3</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="33"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="D22" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="33"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="25"/>
       <c r="E23" s="21"/>
       <c r="F23" s="25"/>
       <c r="G23" s="25"/>
-      <c r="H23" s="33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H23" s="25"/>
+      <c r="I23" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>26</v>
       </c>
@@ -1376,46 +1458,51 @@
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" s="33"/>
-    </row>
-    <row r="25" spans="1:8" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" s="33"/>
+    </row>
+    <row r="25" spans="1:9" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="25"/>
       <c r="E25" s="21"/>
       <c r="F25" s="25"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="33"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H25" s="25"/>
+      <c r="I25" s="33"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="26"/>
       <c r="E26" s="23"/>
       <c r="F26" s="26"/>
       <c r="G26" s="26"/>
-      <c r="H26" s="34"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H26" s="26"/>
+      <c r="I26" s="34"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>13</v>
@@ -1423,7 +1510,7 @@
       <c r="C29" s="17"/>
       <c r="D29" s="12"/>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
@@ -1506,10 +1593,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1521,104 +1608,104 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1626,10 +1713,10 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1637,10 +1724,10 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1648,13 +1735,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1662,10 +1749,10 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1673,10 +1760,10 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1684,10 +1771,10 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1695,10 +1782,10 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1706,10 +1793,10 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1717,10 +1804,10 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1728,32 +1815,87 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
         <v>97</v>
-      </c>
-      <c r="B20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B21" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added first draft of ProcedureRequest and extension based on PlannedCareActivity
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -1212,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated markers, Resource.text and XLS with progress
This concludes the final round of cleanup before going into public review
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Nictiz-STU3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahenket/Development/GitHub/Nictiz/Nictiz-STU3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="-27000" windowWidth="32535" windowHeight="16440"/>
+    <workbookView xWindow="-480" yWindow="-27000" windowWidth="34700" windowHeight="27000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Issues" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$D$44</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1"/>
+  <calcPr calcId="145621" iterate="1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="242">
   <si>
     <t>Patiënt</t>
   </si>
@@ -713,12 +716,54 @@
   </si>
   <si>
     <t>NutritionOrder materials used or needed to perform the order </t>
+  </si>
+  <si>
+    <t>#9824</t>
+  </si>
+  <si>
+    <t>Organization.active description is not clear</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Description in FHIR updated in STU3</t>
+  </si>
+  <si>
+    <t>ZIB-452</t>
+  </si>
+  <si>
+    <t>AfdelingSpecialisme hoort niet thuis in deze ZIB</t>
+  </si>
+  <si>
+    <t>After initial rejection of the issue, it has been reopened with new supporting arguments</t>
+  </si>
+  <si>
+    <t>ZIB-349</t>
+  </si>
+  <si>
+    <t>VIPIndicator uit bouwsteen OverdrachtPatient verwijderd</t>
+  </si>
+  <si>
+    <t>ZIB-501</t>
+  </si>
+  <si>
+    <t>ZIB-502</t>
+  </si>
+  <si>
+    <t>Zorgverlener zou meerdere rollen moeten ondersteunen</t>
+  </si>
+  <si>
+    <t>ZorgverlenerRol hoort niet thuis bij Zorgverlener</t>
+  </si>
+  <si>
+    <t>The ZIB issue is rejected, but because of PractitionerRole in FHIR STU3 is it no longer an issue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1168,13 +1213,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Goed" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="4" builtinId="28"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Ongeldig" xfId="3" builtinId="27"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1478,25 +1523,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="10" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.796875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="79.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.3984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" style="10" customWidth="1"/>
+    <col min="10" max="10" width="21.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
         <v>202</v>
       </c>
@@ -1525,7 +1570,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1591,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>37</v>
       </c>
@@ -1565,7 +1610,7 @@
       <c r="H3" s="22"/>
       <c r="I3" s="64"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>190</v>
       </c>
@@ -1582,7 +1627,7 @@
       <c r="H4" s="18"/>
       <c r="I4" s="63"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -1601,7 +1646,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>2</v>
       </c>
@@ -1620,7 +1665,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1637,7 +1682,7 @@
       <c r="H7" s="18"/>
       <c r="I7" s="63"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1701,7 @@
       </c>
       <c r="I8" s="63"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>193</v>
       </c>
@@ -1675,7 +1720,7 @@
       <c r="H9" s="18"/>
       <c r="I9" s="63"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1739,7 @@
       </c>
       <c r="I10" s="63"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
@@ -1713,7 +1758,7 @@
       </c>
       <c r="I11" s="63"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>6</v>
       </c>
@@ -1732,7 +1777,7 @@
       </c>
       <c r="I12" s="63"/>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>7</v>
       </c>
@@ -1751,7 +1796,7 @@
       </c>
       <c r="I13" s="63"/>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>12</v>
       </c>
@@ -1772,7 +1817,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
@@ -1793,7 +1838,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -1818,7 +1863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>14</v>
       </c>
@@ -1839,7 +1884,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
@@ -1860,7 +1905,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
@@ -1881,7 +1926,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1947,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>10</v>
       </c>
@@ -1925,7 +1970,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
@@ -1946,7 +1991,7 @@
       </c>
       <c r="I22" s="63"/>
     </row>
-    <row r="23" spans="1:9" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>214</v>
       </c>
@@ -1965,7 +2010,7 @@
       <c r="H23" s="18"/>
       <c r="I23" s="63"/>
     </row>
-    <row r="24" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>214</v>
       </c>
@@ -1984,7 +2029,7 @@
       <c r="H24" s="18"/>
       <c r="I24" s="63"/>
     </row>
-    <row r="25" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>214</v>
       </c>
@@ -2003,7 +2048,7 @@
       <c r="H25" s="18"/>
       <c r="I25" s="63"/>
     </row>
-    <row r="26" spans="1:9" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="8" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>214</v>
       </c>
@@ -2022,7 +2067,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="63"/>
     </row>
-    <row r="27" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>214</v>
       </c>
@@ -2039,7 +2084,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="63"/>
     </row>
-    <row r="28" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
@@ -2064,7 +2109,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="42" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>20</v>
       </c>
@@ -2089,7 +2134,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="49" t="s">
         <v>209</v>
       </c>
@@ -2102,7 +2147,7 @@
       <c r="H30" s="55"/>
       <c r="I30" s="65"/>
     </row>
-    <row r="31" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>194</v>
       </c>
@@ -2123,7 +2168,7 @@
       </c>
       <c r="I31" s="63"/>
     </row>
-    <row r="32" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>196</v>
       </c>
@@ -2142,7 +2187,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="63"/>
     </row>
-    <row r="33" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>197</v>
       </c>
@@ -2161,7 +2206,7 @@
       <c r="H33" s="18"/>
       <c r="I33" s="63"/>
     </row>
-    <row r="34" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>201</v>
       </c>
@@ -2180,7 +2225,7 @@
       <c r="H34" s="18"/>
       <c r="I34" s="63"/>
     </row>
-    <row r="35" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>200</v>
       </c>
@@ -2199,7 +2244,7 @@
       <c r="H35" s="18"/>
       <c r="I35" s="63"/>
     </row>
-    <row r="36" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>199</v>
       </c>
@@ -2218,7 +2263,7 @@
       <c r="H36" s="18"/>
       <c r="I36" s="63"/>
     </row>
-    <row r="37" spans="1:9" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="49" t="s">
         <v>208</v>
       </c>
@@ -2231,7 +2276,7 @@
       <c r="H37" s="55"/>
       <c r="I37" s="65"/>
     </row>
-    <row r="38" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
         <v>170</v>
       </c>
@@ -2248,7 +2293,7 @@
       <c r="H38" s="18"/>
       <c r="I38" s="63"/>
     </row>
-    <row r="39" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
         <v>171</v>
       </c>
@@ -2265,7 +2310,7 @@
       <c r="H39" s="18"/>
       <c r="I39" s="63"/>
     </row>
-    <row r="40" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
         <v>178</v>
       </c>
@@ -2282,7 +2327,7 @@
       <c r="H40" s="18"/>
       <c r="I40" s="63"/>
     </row>
-    <row r="41" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
         <v>173</v>
       </c>
@@ -2299,7 +2344,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="63"/>
     </row>
-    <row r="42" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
         <v>174</v>
       </c>
@@ -2316,7 +2361,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="63"/>
     </row>
-    <row r="43" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
         <v>179</v>
       </c>
@@ -2333,7 +2378,7 @@
       <c r="H43" s="18"/>
       <c r="I43" s="63"/>
     </row>
-    <row r="44" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="28" t="s">
         <v>185</v>
       </c>
@@ -2350,7 +2395,7 @@
       <c r="H44" s="18"/>
       <c r="I44" s="63"/>
     </row>
-    <row r="45" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
         <v>176</v>
       </c>
@@ -2367,7 +2412,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="63"/>
     </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="45" t="s">
         <v>177</v>
       </c>
@@ -2452,21 +2497,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.3984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.3984375" customWidth="1"/>
+    <col min="4" max="4" width="24.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>48</v>
       </c>
@@ -2483,157 +2528,163 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B8" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C8" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D8" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E8" s="31" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B9" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C9" t="s">
         <v>182</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E9" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>96</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="F10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>35</v>
       </c>
@@ -2650,7 +2701,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
@@ -2667,7 +2718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>35</v>
       </c>
@@ -2681,7 +2732,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>35</v>
       </c>
@@ -2695,7 +2746,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>35</v>
       </c>
@@ -2712,259 +2763,250 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" t="s">
-        <v>125</v>
+        <v>88</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>6</v>
+        <v>204</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>68</v>
+        <v>90</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
-        <v>7</v>
+        <v>206</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>81</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>146</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>143</v>
-      </c>
-      <c r="E25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="F27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
+        <v>13</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>235</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>236</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>151</v>
@@ -2973,15 +3015,15 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>151</v>
@@ -2990,86 +3032,83 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
-        <v>55</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>163</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
-      </c>
-      <c r="F32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>75</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
-        <v>159</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>158</v>
+        <v>59</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>151</v>
@@ -3078,41 +3117,41 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>164</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
-      </c>
-      <c r="E38" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>167</v>
       </c>
@@ -3126,40 +3165,135 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>225</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
         <v>224</v>
       </c>
       <c r="C40" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>167</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>227</v>
+        <v>80</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>228</v>
+      </c>
+      <c r="C42" t="s">
+        <v>229</v>
+      </c>
+      <c r="D42" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>232</v>
+      </c>
+      <c r="C43" t="s">
+        <v>233</v>
+      </c>
+      <c r="D43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>237</v>
+      </c>
+      <c r="C45" t="s">
+        <v>239</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>238</v>
+      </c>
+      <c r="C46" t="s">
+        <v>240</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
+  <autoFilter ref="A1:D44">
     <sortState ref="A2:D36">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
+  <sortState ref="A2:F44">
+    <sortCondition ref="A2:A44"/>
+    <sortCondition ref="B2:B44"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Medication: aligned MedicationAdministration to ZIBs 2017
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="239">
   <si>
     <t>Patiënt</t>
   </si>
@@ -548,9 +548,6 @@
   </si>
   <si>
     <t>DosageInstructions</t>
-  </si>
-  <si>
-    <t>No formal mapping in profile yet</t>
   </si>
   <si>
     <t>#13459</t>
@@ -1532,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1553,10 +1550,10 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="48" t="s">
         <v>195</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>196</v>
       </c>
       <c r="C1" s="49" t="s">
         <v>34</v>
@@ -1568,10 +1565,10 @@
         <v>39</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H1" s="52" t="s">
         <v>32</v>
@@ -1608,7 +1605,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="70" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="32"/>
@@ -1623,10 +1620,10 @@
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>183</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>184</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="5"/>
@@ -1664,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="5"/>
@@ -1719,7 +1716,7 @@
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>26</v>
@@ -1750,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="62" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G10" s="73"/>
       <c r="H10" s="16"/>
@@ -1878,7 +1875,7 @@
       <c r="F16" s="74"/>
       <c r="G16" s="74"/>
       <c r="H16" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I16" s="16" t="s">
         <v>98</v>
@@ -1900,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G17" s="73"/>
       <c r="H17" s="16"/>
@@ -1960,7 +1957,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
@@ -1974,7 +1971,7 @@
         <v>98</v>
       </c>
       <c r="J20" s="54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
@@ -1998,7 +1995,7 @@
         <v>98</v>
       </c>
       <c r="J21" s="54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -2025,10 +2022,10 @@
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>206</v>
-      </c>
-      <c r="B23" s="58" t="s">
-        <v>207</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5"/>
@@ -2043,10 +2040,10 @@
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24" s="59" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5"/>
@@ -2061,10 +2058,10 @@
     </row>
     <row r="25" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B25" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5"/>
@@ -2074,17 +2071,17 @@
       <c r="F25" s="73"/>
       <c r="G25" s="73"/>
       <c r="H25" s="35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I25" s="16"/>
       <c r="J25" s="54"/>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
@@ -2099,7 +2096,7 @@
     </row>
     <row r="27" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B27" s="69" t="s">
         <v>170</v>
@@ -2110,7 +2107,7 @@
       <c r="F27" s="78"/>
       <c r="G27" s="78"/>
       <c r="H27" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I27" s="16"/>
       <c r="J27" s="54"/>
@@ -2134,7 +2131,7 @@
         <v>98</v>
       </c>
       <c r="J28" s="54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2156,18 +2153,18 @@
         <v>98</v>
       </c>
       <c r="J29" s="54" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="43"/>
       <c r="D30" s="44"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="63"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="63"/>
       <c r="H30" s="46"/>
       <c r="I30" s="46"/>
@@ -2175,20 +2172,20 @@
     </row>
     <row r="31" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E31" s="25"/>
-      <c r="F31" s="64"/>
+      <c r="F31" s="25"/>
       <c r="G31" s="64"/>
       <c r="H31" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I31" s="35" t="s">
         <v>98</v>
@@ -2197,113 +2194,113 @@
     </row>
     <row r="32" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="33"/>
       <c r="D32" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E32" s="25"/>
-      <c r="F32" s="64"/>
+      <c r="F32" s="25"/>
       <c r="G32" s="64"/>
       <c r="H32" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I32" s="16"/>
       <c r="J32" s="54"/>
     </row>
     <row r="33" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B33" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="33"/>
       <c r="D33" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E33" s="25"/>
-      <c r="F33" s="64"/>
+      <c r="F33" s="25"/>
       <c r="G33" s="64"/>
       <c r="H33" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I33" s="16"/>
       <c r="J33" s="54"/>
     </row>
     <row r="34" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E34" s="25"/>
-      <c r="F34" s="64"/>
+      <c r="F34" s="25"/>
       <c r="G34" s="64"/>
       <c r="H34" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I34" s="16"/>
       <c r="J34" s="54"/>
     </row>
     <row r="35" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B35" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="33"/>
       <c r="D35" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E35" s="25"/>
-      <c r="F35" s="64"/>
+      <c r="F35" s="25"/>
       <c r="G35" s="64"/>
       <c r="H35" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I35" s="16"/>
       <c r="J35" s="54"/>
     </row>
     <row r="36" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="33"/>
       <c r="D36" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E36" s="25"/>
-      <c r="F36" s="64"/>
+      <c r="F36" s="25"/>
       <c r="G36" s="64"/>
       <c r="H36" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I36" s="16"/>
       <c r="J36" s="54"/>
     </row>
     <row r="37" spans="1:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="43"/>
       <c r="D37" s="44"/>
       <c r="E37" s="45"/>
-      <c r="F37" s="63"/>
+      <c r="F37" s="45"/>
       <c r="G37" s="63"/>
       <c r="H37" s="46"/>
       <c r="I37" s="46"/>
@@ -2318,12 +2315,12 @@
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="65"/>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="5"/>
       <c r="G38" s="65"/>
-      <c r="H38" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H38" s="22"/>
       <c r="I38" s="16"/>
       <c r="J38" s="54"/>
     </row>
@@ -2339,11 +2336,9 @@
       <c r="E39" s="3">
         <v>1</v>
       </c>
-      <c r="F39" s="66"/>
+      <c r="F39" s="5"/>
       <c r="G39" s="66"/>
-      <c r="H39" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H39" s="22"/>
       <c r="I39" s="16"/>
       <c r="J39" s="54"/>
     </row>
@@ -2359,11 +2354,9 @@
       <c r="E40" s="3">
         <v>1</v>
       </c>
-      <c r="F40" s="66"/>
+      <c r="F40" s="5"/>
       <c r="G40" s="66"/>
-      <c r="H40" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H40" s="22"/>
       <c r="I40" s="16"/>
       <c r="J40" s="54"/>
     </row>
@@ -2379,11 +2372,9 @@
       <c r="E41" s="3">
         <v>1</v>
       </c>
-      <c r="F41" s="66"/>
+      <c r="F41" s="5"/>
       <c r="G41" s="66"/>
-      <c r="H41" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H41" s="22"/>
       <c r="I41" s="16"/>
       <c r="J41" s="54"/>
     </row>
@@ -2399,11 +2390,9 @@
       <c r="E42" s="3">
         <v>1</v>
       </c>
-      <c r="F42" s="66"/>
+      <c r="F42" s="5"/>
       <c r="G42" s="66"/>
-      <c r="H42" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H42" s="22"/>
       <c r="I42" s="16"/>
       <c r="J42" s="54"/>
     </row>
@@ -2412,34 +2401,30 @@
         <v>174</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5"/>
       <c r="E43" s="26"/>
-      <c r="F43" s="66"/>
+      <c r="F43" s="5"/>
       <c r="G43" s="66"/>
-      <c r="H43" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H43" s="22"/>
       <c r="I43" s="16"/>
       <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5"/>
       <c r="E44" s="26"/>
-      <c r="F44" s="66"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="66"/>
-      <c r="H44" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H44" s="22"/>
       <c r="I44" s="16"/>
       <c r="J44" s="54"/>
     </row>
@@ -2453,11 +2438,9 @@
       <c r="C45" s="2"/>
       <c r="D45" s="5"/>
       <c r="E45" s="26"/>
-      <c r="F45" s="66"/>
+      <c r="F45" s="5"/>
       <c r="G45" s="66"/>
-      <c r="H45" s="22" t="s">
-        <v>175</v>
-      </c>
+      <c r="H45" s="22"/>
       <c r="I45" s="16"/>
       <c r="J45" s="54"/>
     </row>
@@ -2471,11 +2454,9 @@
       <c r="C46" s="18"/>
       <c r="D46" s="60"/>
       <c r="E46" s="14"/>
-      <c r="F46" s="67"/>
+      <c r="F46" s="60"/>
       <c r="G46" s="67"/>
-      <c r="H46" s="39" t="s">
-        <v>175</v>
-      </c>
+      <c r="H46" s="39"/>
       <c r="I46" s="17"/>
       <c r="J46" s="57"/>
     </row>
@@ -2705,13 +2686,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9" t="s">
         <v>176</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>177</v>
-      </c>
-      <c r="E9" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2832,13 +2813,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" t="s">
         <v>214</v>
-      </c>
-      <c r="B17" t="s">
-        <v>213</v>
-      </c>
-      <c r="C17" t="s">
-        <v>215</v>
       </c>
       <c r="D17" t="s">
         <v>137</v>
@@ -2863,7 +2844,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B19" t="s">
         <v>71</v>
@@ -2897,7 +2878,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
         <v>157</v>
@@ -2982,7 +2963,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B26" t="s">
         <v>117</v>
@@ -3053,10 +3034,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" t="s">
         <v>224</v>
-      </c>
-      <c r="C30" t="s">
-        <v>225</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>147</v>
@@ -3220,10 +3201,10 @@
         <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>137</v>
@@ -3251,16 +3232,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>216</v>
+      </c>
+      <c r="C42" t="s">
         <v>217</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>218</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>219</v>
-      </c>
-      <c r="E42" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -3268,16 +3249,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>220</v>
+      </c>
+      <c r="C43" t="s">
         <v>221</v>
-      </c>
-      <c r="C43" t="s">
-        <v>222</v>
       </c>
       <c r="D43" t="s">
         <v>145</v>
       </c>
       <c r="E43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -3305,16 +3286,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D45" t="s">
         <v>139</v>
       </c>
       <c r="E45" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3322,27 +3303,27 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47" t="s">
+        <v>230</v>
+      </c>
+      <c r="C47" t="s">
         <v>232</v>
-      </c>
-      <c r="B47" t="s">
-        <v>231</v>
-      </c>
-      <c r="C47" t="s">
-        <v>233</v>
       </c>
       <c r="D47" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Vital Signs: first commit of derived vital signs profiles
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="244">
   <si>
     <t>Patiënt</t>
   </si>
@@ -586,18 +586,12 @@
     <t>Bloeddruk</t>
   </si>
   <si>
-    <t>http://www.hl7.org/fhir/STU3/observation-vitalsigns.html</t>
-  </si>
-  <si>
     <t>Lichaamsgewicht</t>
   </si>
   <si>
     <t>Lichaamslengte</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Polsfrequentie</t>
   </si>
   <si>
@@ -740,6 +734,27 @@
   </si>
   <si>
     <t>V3.1</t>
+  </si>
+  <si>
+    <t>GlasgowComaScale</t>
+  </si>
+  <si>
+    <t>Hartfrequentie</t>
+  </si>
+  <si>
+    <t>Pijnscore</t>
+  </si>
+  <si>
+    <t>Ademhaling</t>
+  </si>
+  <si>
+    <t>Concepten to do: CuffType, DiastolicEndpoint, Position</t>
+  </si>
+  <si>
+    <t>Geen bijzonderheden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concept to do: ExtraOxygenAdministration </t>
   </si>
 </sst>
 </file>
@@ -901,7 +916,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -958,17 +973,6 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -1053,13 +1057,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1077,22 +1081,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1104,33 +1107,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,27 +1143,27 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1172,10 +1175,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1190,25 +1193,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1527,10 +1530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1540,8 +1543,8 @@
     <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="68" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="68" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="67" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="67" customWidth="1"/>
     <col min="8" max="8" width="54.85546875" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" style="7" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" style="9" customWidth="1"/>
@@ -1549,34 +1552,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="A1" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="80" t="s">
-        <v>237</v>
-      </c>
-      <c r="G1" s="51" t="s">
+      <c r="F1" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="G1" s="50" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="52" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1584,45 +1587,45 @@
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="11"/>
-      <c r="D2" s="61"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="53" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="69" t="s">
         <v>184</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="32"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="55"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="54"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>183</v>
       </c>
       <c r="C4" s="2"/>
@@ -1630,17 +1633,17 @@
       <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="54"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="12"/>
@@ -1648,11 +1651,11 @@
       <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="54" t="s">
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="53" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1660,7 +1663,7 @@
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>179</v>
       </c>
       <c r="C6" s="12"/>
@@ -1668,11 +1671,11 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="54" t="s">
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="53" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1680,7 +1683,7 @@
       <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="12"/>
@@ -1688,17 +1691,17 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="54"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="2"/>
@@ -1706,19 +1709,19 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16" t="s">
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="54"/>
+      <c r="J8" s="53"/>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="2"/>
@@ -1726,19 +1729,19 @@
       <c r="E9" s="3">
         <v>18</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="22" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="54"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2"/>
@@ -1746,21 +1749,21 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="62" t="s">
-        <v>238</v>
-      </c>
-      <c r="G10" s="73"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16" t="s">
+      <c r="F10" s="61" t="s">
+        <v>236</v>
+      </c>
+      <c r="G10" s="72"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J10" s="54"/>
+      <c r="J10" s="53"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
@@ -1768,19 +1771,19 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16" t="s">
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J11" s="54"/>
+      <c r="J11" s="53"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2"/>
@@ -1788,19 +1791,19 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16" t="s">
+      <c r="F12" s="72"/>
+      <c r="G12" s="72"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J12" s="54"/>
+      <c r="J12" s="53"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
@@ -1808,19 +1811,19 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16" t="s">
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J13" s="54"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="2"/>
@@ -1828,13 +1831,13 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16" t="s">
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="54" t="s">
+      <c r="J14" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1842,7 +1845,7 @@
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2"/>
@@ -1850,13 +1853,13 @@
       <c r="E15" s="3">
         <v>2</v>
       </c>
-      <c r="F15" s="73"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16" t="s">
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="54" t="s">
+      <c r="J15" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1864,7 +1867,7 @@
       <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="2"/>
@@ -1872,15 +1875,15 @@
       <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="I16" s="16" t="s">
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="I16" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="54" t="s">
+      <c r="J16" s="53" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1888,7 +1891,7 @@
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2"/>
@@ -1896,15 +1899,15 @@
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="G17" s="73"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16" t="s">
+      <c r="F17" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="G17" s="72"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J17" s="54" t="s">
+      <c r="J17" s="53" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1912,7 +1915,7 @@
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="2"/>
@@ -1920,13 +1923,13 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16" t="s">
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J18" s="54" t="s">
+      <c r="J18" s="53" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1934,7 +1937,7 @@
       <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="2"/>
@@ -1942,13 +1945,13 @@
       <c r="E19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16" t="s">
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="53" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1956,29 +1959,29 @@
       <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>211</v>
+      <c r="B20" s="28" t="s">
+        <v>209</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
       <c r="E20" s="3">
         <v>3</v>
       </c>
-      <c r="F20" s="77"/>
-      <c r="G20" s="77"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16" t="s">
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="54" t="s">
-        <v>203</v>
+      <c r="J20" s="53" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="2"/>
@@ -1986,23 +1989,23 @@
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="73"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="31" t="s">
+      <c r="F21" s="72"/>
+      <c r="G21" s="78"/>
+      <c r="H21" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J21" s="54" t="s">
-        <v>204</v>
+      <c r="J21" s="53" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2"/>
@@ -2010,113 +2013,113 @@
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="16" t="s">
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="54"/>
+      <c r="J22" s="53"/>
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B23" s="58" t="s">
-        <v>206</v>
+        <v>203</v>
+      </c>
+      <c r="B23" s="57" t="s">
+        <v>204</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5"/>
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="54"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="53"/>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="58" t="s">
         <v>205</v>
-      </c>
-      <c r="B24" s="59" t="s">
-        <v>207</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5"/>
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="54"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="53"/>
     </row>
     <row r="25" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" s="59" t="s">
-        <v>208</v>
+        <v>203</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>206</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="I25" s="16"/>
-      <c r="J25" s="54"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="I25" s="15"/>
+      <c r="J25" s="53"/>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B26" s="59" t="s">
-        <v>209</v>
+        <v>203</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>207</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="54"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="53"/>
     </row>
     <row r="27" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="B27" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="68" t="s">
         <v>170</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="5"/>
       <c r="E27" s="13"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="35" t="s">
-        <v>234</v>
-      </c>
-      <c r="I27" s="16"/>
-      <c r="J27" s="54"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="I27" s="15"/>
+      <c r="J27" s="53"/>
     </row>
     <row r="28" spans="1:10" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="2"/>
@@ -2124,21 +2127,21 @@
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16" t="s">
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J28" s="54" t="s">
-        <v>201</v>
+      <c r="J28" s="53" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="2"/>
@@ -2146,340 +2149,394 @@
       <c r="E29" s="3">
         <v>1</v>
       </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="16" t="s">
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="J29" s="54" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="J29" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="56"/>
+    </row>
+    <row r="30" spans="1:10" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="55"/>
     </row>
     <row r="31" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="34" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="I31" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="J31" s="53"/>
+    </row>
+    <row r="32" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="32"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="53"/>
+    </row>
+    <row r="33" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="32"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="53"/>
+    </row>
+    <row r="34" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="32"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="I34" s="15"/>
+      <c r="J34" s="53"/>
+    </row>
+    <row r="35" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" s="54"/>
-    </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="B32" s="29" t="s">
+      <c r="B35" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="54"/>
-    </row>
-    <row r="33" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="C35" s="32"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="15"/>
+      <c r="J35" s="53"/>
+    </row>
+    <row r="36" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B36" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="54"/>
-    </row>
-    <row r="34" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="B34" s="29" t="s">
+      <c r="C36" s="32"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="53"/>
+    </row>
+    <row r="37" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I34" s="16"/>
-      <c r="J34" s="54"/>
-    </row>
-    <row r="35" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="B35" s="29" t="s">
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="53"/>
+    </row>
+    <row r="38" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I35" s="16"/>
-      <c r="J35" s="54"/>
-    </row>
-    <row r="36" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="B36" s="29" t="s">
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="53"/>
+    </row>
+    <row r="39" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="B39" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="33"/>
-      <c r="D36" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="I36" s="16"/>
-      <c r="J36" s="54"/>
-    </row>
-    <row r="37" spans="1:10" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="56"/>
-    </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="53"/>
+    </row>
+    <row r="40" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="53"/>
+    </row>
+    <row r="41" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="53"/>
+    </row>
+    <row r="42" spans="1:10" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" s="41"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="55"/>
+    </row>
+    <row r="43" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>165</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="3">
-        <v>1</v>
-      </c>
-      <c r="F38" s="5"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="54"/>
-    </row>
-    <row r="39" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="3">
-        <v>1</v>
-      </c>
-      <c r="F39" s="5"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="54"/>
-    </row>
-    <row r="40" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="3">
-        <v>1</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="54"/>
-    </row>
-    <row r="41" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="3">
-        <v>1</v>
-      </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="22"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="54"/>
-    </row>
-    <row r="42" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>170</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="3">
-        <v>1</v>
-      </c>
-      <c r="F42" s="5"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="22"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="54"/>
-    </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>180</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="26"/>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
       <c r="F43" s="5"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="54"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="53"/>
     </row>
     <row r="44" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>181</v>
+      <c r="A44" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>167</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="26"/>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="16"/>
-      <c r="J44" s="54"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>171</v>
+      <c r="A45" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>170</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="26"/>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
       <c r="F45" s="5"/>
-      <c r="G45" s="66"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="16"/>
-      <c r="J45" s="54"/>
-    </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
+      <c r="G45" s="65"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="53"/>
+    </row>
+    <row r="46" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="53"/>
+    </row>
+    <row r="47" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="53"/>
+    </row>
+    <row r="48" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="53"/>
+    </row>
+    <row r="49" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="53"/>
+    </row>
+    <row r="50" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="53"/>
+    </row>
+    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="57"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="9"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="9"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="9"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="9"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" s="9"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="9"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="9"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="59"/>
+      <c r="E51" s="59">
+        <v>1</v>
+      </c>
+      <c r="F51" s="59"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="56"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B59" s="9"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="9"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B61" s="9"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
@@ -2516,6 +2573,18 @@
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" s="9"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="9"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="9"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="9"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2543,19 +2612,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>149</v>
       </c>
     </row>
@@ -2665,19 +2734,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2719,7 +2788,7 @@
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>108</v>
       </c>
       <c r="C11" t="s">
@@ -2736,7 +2805,7 @@
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>103</v>
       </c>
       <c r="C12" t="s">
@@ -2753,7 +2822,7 @@
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>109</v>
       </c>
       <c r="C13" t="s">
@@ -2767,7 +2836,7 @@
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>104</v>
       </c>
       <c r="C14" t="s">
@@ -2813,13 +2882,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" t="s">
         <v>212</v>
-      </c>
-      <c r="C17" t="s">
-        <v>214</v>
       </c>
       <c r="D17" t="s">
         <v>137</v>
@@ -2844,7 +2913,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
         <v>71</v>
@@ -2878,7 +2947,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
         <v>157</v>
@@ -2963,7 +3032,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
         <v>117</v>
@@ -3034,10 +3103,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>147</v>
@@ -3201,10 +3270,10 @@
         <v>163</v>
       </c>
       <c r="B40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>137</v>
@@ -3232,16 +3301,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>214</v>
+      </c>
+      <c r="C42" t="s">
+        <v>215</v>
+      </c>
+      <c r="D42" t="s">
         <v>216</v>
       </c>
-      <c r="C42" t="s">
+      <c r="E42" t="s">
         <v>217</v>
-      </c>
-      <c r="D42" t="s">
-        <v>218</v>
-      </c>
-      <c r="E42" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -3249,16 +3318,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D43" t="s">
         <v>145</v>
       </c>
       <c r="E43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -3286,16 +3355,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
+        <v>223</v>
+      </c>
+      <c r="C45" t="s">
         <v>225</v>
-      </c>
-      <c r="C45" t="s">
-        <v>227</v>
       </c>
       <c r="D45" t="s">
         <v>139</v>
       </c>
       <c r="E45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3303,27 +3372,27 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>224</v>
+      </c>
+      <c r="C46" t="s">
         <v>226</v>
-      </c>
-      <c r="C46" t="s">
-        <v>228</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B47" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" t="s">
         <v>230</v>
-      </c>
-      <c r="C47" t="s">
-        <v>232</v>
       </c>
       <c r="D47" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Updated validtionstatus of resources in the .xlsx
</commit_message>
<xml_diff>
--- a/Progress - BGZ to FHIR.xlsx
+++ b/Progress - BGZ to FHIR.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="-27000" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="-480" yWindow="-27000" windowWidth="21810" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$D$44</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="145621" iterate="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="269">
   <si>
     <t>Patiënt</t>
   </si>
@@ -313,9 +313,6 @@
     <t>Add a note element to NutritionOrder </t>
   </si>
   <si>
-    <t xml:space="preserve">Not everything is profiled yet, example can be improved. This whole recource needs attention! gForge #13294 - </t>
-  </si>
-  <si>
     <t>Issues? FHIR / ZIB</t>
   </si>
   <si>
@@ -523,27 +520,18 @@
     <t>Medication</t>
   </si>
   <si>
-    <t>MedicationUsage</t>
-  </si>
-  <si>
     <t>MedicationStatement</t>
   </si>
   <si>
     <t>MedicationDispense</t>
   </si>
   <si>
-    <t>MedicationDispenseRequest</t>
-  </si>
-  <si>
     <t>MedicationRequest</t>
   </si>
   <si>
     <t>MedicationAdministration</t>
   </si>
   <si>
-    <t>MedicationAdministrationAgreement</t>
-  </si>
-  <si>
     <t>MedicationAgreement</t>
   </si>
   <si>
@@ -592,9 +580,6 @@
     <t>Lichaamslengte</t>
   </si>
   <si>
-    <t>Polsfrequentie</t>
-  </si>
-  <si>
     <t>O2Saturatie</t>
   </si>
   <si>
@@ -649,9 +634,6 @@
     <t>Appointment</t>
   </si>
   <si>
-    <t xml:space="preserve">Similar as ZIB Vaccination </t>
-  </si>
-  <si>
     <t xml:space="preserve">Coverage / Organization / Patient </t>
   </si>
   <si>
@@ -721,47 +703,140 @@
     <t>Fixed valueset VerrichtingTypeCodelijst to ZIB version 3.0 because of invalid valueset in version 1.2.</t>
   </si>
   <si>
-    <t>Similar as MedicationAgreement</t>
-  </si>
-  <si>
     <t>Validated?</t>
   </si>
   <si>
-    <t>v3,1</t>
-  </si>
-  <si>
-    <t>Checked against ZIB 2017 excl valuesets</t>
-  </si>
-  <si>
-    <t>V3.1</t>
-  </si>
-  <si>
-    <t>GlasgowComaScale</t>
-  </si>
-  <si>
     <t>Hartfrequentie</t>
   </si>
   <si>
-    <t>Pijnscore</t>
-  </si>
-  <si>
-    <t>Ademhaling</t>
-  </si>
-  <si>
-    <t>Concepten to do: CuffType, DiastolicEndpoint, Position</t>
-  </si>
-  <si>
-    <t>Geen bijzonderheden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concept to do: ExtraOxygenAdministration </t>
+    <t>Eigen derived</t>
+  </si>
+  <si>
+    <t>MedicationUse</t>
+  </si>
+  <si>
+    <t>AdministrationAgreement</t>
+  </si>
+  <si>
+    <t>DispenseRequest</t>
+  </si>
+  <si>
+    <t>Dispense</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/tobaccouse-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/RelatedPerson-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/nl-core-practitionerrole-example-1 https://simplifier.net/NictizSTU3/nl-core-practitioner-example-1</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/AllergyIntolerance-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/zib-alcoholuse-example/~examples</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/zib-livingsituation-exmaple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;!-- Correcct terminology needed. Code is now used for TypeOfTobaccoUsed and Amount --&gt;</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Encounter-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Condition-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Procedure-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Flag-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Immunization-example https://simplifier.net/NictizSTU3/ImmunizationRecommendation-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Device-example  https://simplifier.net/NictizSTU3/DeviceUseStatement-example/~xml</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/ui/$validate?fileId=22967</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/NutritionOrder-example/~overview</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/zib-functionalormentalstatus-example/~examples</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/ProcedureRequest-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/ui/$validate?fileId=23366</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/ImmunizationRecommendation-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Appointment-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationRequest-example-3</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Consent-example2/~rendered</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Consent-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationUse-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationDispense-example-1</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationRequest-example</t>
+  </si>
+  <si>
+    <t>Included in other examples</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationAdministration-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/MedicationDispense-example-2</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Medication-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Observation-example151 https://simplifier.net/NictizSTU3/DiagnosticReport-example</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/nl-core-patient-example-1</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/ui/$validate?fileId=23023</t>
+  </si>
+  <si>
+    <t>https://simplifier.net/NictizSTU3/Observation-example</t>
+  </si>
+  <si>
+    <t>Mostly validator issues - resolved with the new deploy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -862,20 +937,32 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -901,12 +988,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -1057,7 +1138,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -1077,7 +1158,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
@@ -1093,7 +1173,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1111,36 +1190,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1149,7 +1224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1166,59 +1241,51 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1530,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1543,107 +1610,106 @@
     <col min="3" max="3" width="9" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="67" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="67" customWidth="1"/>
-    <col min="8" max="8" width="54.85546875" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="59" style="58" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" s="48" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="79" t="s">
-        <v>235</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>233</v>
-      </c>
-      <c r="H1" s="51" t="s">
+      <c r="F1" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="G1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="J1" s="52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="H1" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="11"/>
-      <c r="D2" s="60"/>
+      <c r="D2" s="56"/>
       <c r="E2" s="4">
         <v>1</v>
       </c>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="F2" s="61" t="s">
+        <v>265</v>
+      </c>
+      <c r="G2" s="13"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="53" t="s">
+      <c r="I2" s="49" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="69" t="s">
-        <v>184</v>
+      <c r="B3" s="60" t="s">
+        <v>180</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="31"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="54"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>183</v>
+      <c r="F3" s="62" t="s">
+        <v>265</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="50"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>179</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="5"/>
       <c r="E4" s="3">
         <v>1</v>
       </c>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="53"/>
-    </row>
-    <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F4" s="63" t="s">
+        <v>265</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="49"/>
+    </row>
+    <row r="5" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="12"/>
@@ -1651,39 +1717,41 @@
       <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="53" t="s">
+      <c r="F5" s="63" t="s">
+        <v>266</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="49" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="28" t="s">
-        <v>179</v>
+      <c r="B6" s="26" t="s">
+        <v>175</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="5"/>
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="53" t="s">
+      <c r="F6" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="49" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="12"/>
@@ -1691,17 +1759,18 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="53"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="49"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C8" s="2"/>
@@ -1709,19 +1778,20 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J8" s="53"/>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="B9" s="29" t="s">
+      <c r="F8" s="64" t="s">
+        <v>237</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I8" s="49"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="2"/>
@@ -1729,19 +1799,20 @@
       <c r="E9" s="3">
         <v>18</v>
       </c>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="53"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F9" s="63" t="s">
+        <v>264</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="49"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="2"/>
@@ -1749,21 +1820,20 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="F10" s="61" t="s">
-        <v>236</v>
-      </c>
-      <c r="G10" s="72"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J10" s="53"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F10" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="49"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2"/>
@@ -1771,19 +1841,22 @@
       <c r="E11" s="3">
         <v>1</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11" s="53"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F11" s="64" t="s">
+        <v>234</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="49"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2"/>
@@ -1791,19 +1864,20 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="72"/>
-      <c r="G12" s="72"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J12" s="53"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F12" s="57" t="s">
+        <v>267</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="49"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="2"/>
@@ -1811,19 +1885,20 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J13" s="53"/>
-    </row>
-    <row r="14" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F13" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="49"/>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="2"/>
@@ -1831,21 +1906,22 @@
       <c r="E14" s="3">
         <v>2</v>
       </c>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" s="53" t="s">
+      <c r="F14" s="63" t="s">
+        <v>241</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I14" s="49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2"/>
@@ -1853,21 +1929,22 @@
       <c r="E15" s="3">
         <v>2</v>
       </c>
-      <c r="F15" s="72"/>
-      <c r="G15" s="72"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="53" t="s">
+      <c r="F15" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="2"/>
@@ -1875,23 +1952,24 @@
       <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="53" t="s">
+      <c r="F16" s="64" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="2"/>
@@ -1899,23 +1977,22 @@
       <c r="E17" s="3">
         <v>1</v>
       </c>
-      <c r="F17" s="61" t="s">
-        <v>234</v>
-      </c>
-      <c r="G17" s="72"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J17" s="53" t="s">
+      <c r="F17" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="2"/>
@@ -1923,21 +2000,22 @@
       <c r="E18" s="3">
         <v>2</v>
       </c>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J18" s="53" t="s">
+      <c r="F18" s="63" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" s="49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="27" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="2"/>
@@ -1945,43 +2023,45 @@
       <c r="E19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J19" s="53" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="F19" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I19" s="49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>209</v>
+      <c r="B20" s="26" t="s">
+        <v>203</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
       <c r="E20" s="3">
         <v>3</v>
       </c>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J20" s="53" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="F20" s="63" t="s">
+        <v>247</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C21" s="2"/>
@@ -1989,23 +2069,22 @@
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="72"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="53" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F21" s="65" t="s">
+        <v>248</v>
+      </c>
+      <c r="G21" s="28"/>
+      <c r="H21" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I21" s="49" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="27" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2"/>
@@ -2013,113 +2092,117 @@
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="I22" s="15" t="s">
+      <c r="F22" s="64" t="s">
+        <v>249</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="J22" s="53"/>
-    </row>
-    <row r="23" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="H22" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="49"/>
+    </row>
+    <row r="23" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B23" s="57" t="s">
-        <v>204</v>
+        <v>198</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>199</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5"/>
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="53"/>
-    </row>
-    <row r="24" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" s="58" t="s">
-        <v>205</v>
+      <c r="F23" s="64" t="s">
+        <v>250</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="49"/>
+    </row>
+    <row r="24" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="54" t="s">
+        <v>200</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5"/>
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="53"/>
-    </row>
-    <row r="25" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F24" s="64" t="s">
+        <v>251</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="49"/>
+    </row>
+    <row r="25" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B25" s="58" t="s">
-        <v>206</v>
+        <v>198</v>
+      </c>
+      <c r="B25" s="54" t="s">
+        <v>201</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5"/>
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="53"/>
-    </row>
-    <row r="26" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F25" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="G25" s="31"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="49"/>
+    </row>
+    <row r="26" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B26" s="58" t="s">
-        <v>207</v>
+        <v>198</v>
+      </c>
+      <c r="B26" s="54" t="s">
+        <v>202</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="E26" s="3">
         <v>1</v>
       </c>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="53"/>
-    </row>
-    <row r="27" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F26" s="64" t="s">
+        <v>253</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="49"/>
+    </row>
+    <row r="27" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="B27" s="68" t="s">
-        <v>170</v>
+        <v>198</v>
+      </c>
+      <c r="B27" s="59" t="s">
+        <v>167</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="53"/>
-    </row>
-    <row r="28" spans="1:10" ht="39" x14ac:dyDescent="0.25">
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="64" t="s">
+        <v>254</v>
+      </c>
+      <c r="G27" s="31"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="49"/>
+    </row>
+    <row r="28" spans="1:9" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="2"/>
@@ -2127,21 +2210,22 @@
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J28" s="53" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="F28" s="64" t="s">
+        <v>255</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I28" s="49" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="35" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="2"/>
@@ -2149,394 +2233,333 @@
       <c r="E29" s="3">
         <v>1</v>
       </c>
-      <c r="F29" s="73"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J29" s="53" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>198</v>
-      </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="55"/>
-    </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="F29" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="G29" s="31"/>
+      <c r="H29" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I29" s="49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="51"/>
+    </row>
+    <row r="31" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="I31" s="49"/>
+    </row>
+    <row r="32" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="49"/>
+    </row>
+    <row r="33" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="49"/>
+    </row>
+    <row r="34" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B34" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="I31" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" s="53"/>
-    </row>
-    <row r="32" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="B32" s="28" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="49"/>
+    </row>
+    <row r="35" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="53"/>
-    </row>
-    <row r="33" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" s="28" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="49"/>
+    </row>
+    <row r="36" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="53"/>
-    </row>
-    <row r="34" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="53"/>
-    </row>
-    <row r="35" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="53"/>
-    </row>
-    <row r="36" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="53"/>
-    </row>
-    <row r="37" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
-        <v>237</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="53"/>
-    </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="53"/>
-    </row>
-    <row r="39" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="53"/>
-    </row>
-    <row r="40" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="15"/>
-      <c r="J40" s="53"/>
-    </row>
-    <row r="41" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="15"/>
-      <c r="J41" s="53"/>
-    </row>
-    <row r="42" spans="1:10" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="B42" s="41"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="55"/>
-    </row>
-    <row r="43" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="C36" s="23"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="49"/>
+    </row>
+    <row r="37" spans="1:9" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="41"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="51"/>
+    </row>
+    <row r="38" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="68" t="s">
+        <v>263</v>
+      </c>
+      <c r="G38" s="72" t="s">
+        <v>268</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="49"/>
+    </row>
+    <row r="39" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="26" t="s">
         <v>165</v>
       </c>
-      <c r="B43" s="28" t="s">
-        <v>165</v>
+      <c r="C39" s="2"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="69" t="s">
+        <v>257</v>
+      </c>
+      <c r="G39" s="72"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="49"/>
+    </row>
+    <row r="40" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="G40" s="72"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="49"/>
+    </row>
+    <row r="41" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="70" t="s">
+        <v>258</v>
+      </c>
+      <c r="G41" s="72"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="49"/>
+    </row>
+    <row r="42" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="G42" s="72"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="49"/>
+    </row>
+    <row r="43" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>176</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="3">
-        <v>1</v>
-      </c>
-      <c r="F43" s="5"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="53"/>
-    </row>
-    <row r="44" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="B44" s="28" t="s">
-        <v>167</v>
+      <c r="E43" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F43" s="69"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="49"/>
+    </row>
+    <row r="44" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>177</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="3">
-        <v>1</v>
-      </c>
-      <c r="F44" s="5"/>
-      <c r="G44" s="65"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="53"/>
-    </row>
-    <row r="45" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>170</v>
+      <c r="E44" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44" s="69"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="49"/>
+    </row>
+    <row r="45" spans="1:9" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="5"/>
       <c r="E45" s="3">
         <v>1</v>
       </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="53"/>
-    </row>
-    <row r="46" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="3">
+      <c r="F45" s="69" t="s">
+        <v>261</v>
+      </c>
+      <c r="G45" s="72"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="49"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55">
         <v>1</v>
       </c>
-      <c r="F46" s="5"/>
-      <c r="G46" s="65"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="53"/>
-    </row>
-    <row r="47" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="3">
-        <v>1</v>
-      </c>
-      <c r="F47" s="5"/>
-      <c r="G47" s="65"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="53"/>
-    </row>
-    <row r="48" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="53"/>
-    </row>
-    <row r="49" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>181</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="53"/>
-    </row>
-    <row r="50" spans="1:10" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="53"/>
-    </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="59"/>
-      <c r="E51" s="59">
-        <v>1</v>
-      </c>
-      <c r="F51" s="59"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="56"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="9"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="9"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="9"/>
+      <c r="F46" s="71" t="s">
+        <v>262</v>
+      </c>
+      <c r="G46" s="73"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="52"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="9"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="9"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="9"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="9"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="9"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="9"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="9"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="9"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" s="9"/>
@@ -2571,27 +2594,16 @@
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" s="9"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="9"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="9"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="9"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="9"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="9"/>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G38:G46"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" display="http://example.org/bodysitecode -&gt; what to do with it?"/>
+    <hyperlink ref="G9" r:id="rId1" display="http://example.org/bodysitecode -&gt; what to do with it?"/>
+    <hyperlink ref="F17" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2612,20 +2624,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="18" t="s">
-        <v>149</v>
+      <c r="E1" s="17" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -2639,10 +2651,10 @@
         <v>76</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2656,13 +2668,13 @@
         <v>72</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2676,10 +2688,10 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
         <v>143</v>
-      </c>
-      <c r="E4" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2693,10 +2705,10 @@
         <v>55</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2710,10 +2722,10 @@
         <v>56</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -2727,27 +2739,27 @@
         <v>57</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>124</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2755,13 +2767,13 @@
         <v>25</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2775,75 +2787,75 @@
         <v>75</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>108</v>
+      <c r="B11" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>103</v>
+      <c r="B12" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>109</v>
+      <c r="B13" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
         <v>104</v>
       </c>
-      <c r="C14" t="s">
-        <v>105</v>
-      </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2851,16 +2863,16 @@
         <v>35</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
         <v>110</v>
       </c>
-      <c r="C15" t="s">
-        <v>111</v>
-      </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2874,24 +2886,24 @@
         <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B17" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2905,15 +2917,15 @@
         <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B19" t="s">
         <v>71</v>
@@ -2922,10 +2934,10 @@
         <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -2939,44 +2951,44 @@
         <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" t="s">
         <v>153</v>
       </c>
-      <c r="C22" t="s">
-        <v>154</v>
-      </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -2990,10 +3002,10 @@
         <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3007,10 +3019,10 @@
         <v>85</v>
       </c>
       <c r="D24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3024,27 +3036,27 @@
         <v>80</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3052,16 +3064,16 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3075,10 +3087,10 @@
         <v>95</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3092,10 +3104,10 @@
         <v>83</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3103,16 +3115,16 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C30" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3120,33 +3132,33 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" t="s">
+        <v>127</v>
+      </c>
+      <c r="E32" t="s">
         <v>160</v>
-      </c>
-      <c r="B32" t="s">
-        <v>158</v>
-      </c>
-      <c r="C32" t="s">
-        <v>159</v>
-      </c>
-      <c r="D32" t="s">
-        <v>128</v>
-      </c>
-      <c r="E32" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3160,10 +3172,10 @@
         <v>93</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -3177,10 +3189,10 @@
         <v>77</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -3194,10 +3206,10 @@
         <v>74</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3211,10 +3223,10 @@
         <v>58</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3228,55 +3240,55 @@
         <v>59</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" t="s">
         <v>120</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>121</v>
       </c>
-      <c r="C38" t="s">
-        <v>122</v>
-      </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" t="s">
+        <v>161</v>
+      </c>
+      <c r="C39" t="s">
         <v>163</v>
       </c>
-      <c r="B39" t="s">
-        <v>162</v>
-      </c>
-      <c r="C39" t="s">
-        <v>164</v>
-      </c>
       <c r="D39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B40" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C40" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -3290,10 +3302,10 @@
         <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -3301,16 +3313,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="C42" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D42" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E42" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -3318,16 +3330,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C43" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -3335,19 +3347,19 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" t="s">
         <v>112</v>
       </c>
-      <c r="C44" t="s">
-        <v>113</v>
-      </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -3355,16 +3367,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C45" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3372,30 +3384,30 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C46" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B47" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C47" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>